<commit_message>
Acrescentei o caso semifinal na funcao de verossimilhanca, e atualizei o banco de dados com jogos das ligas OPL,TCL,LJL E LLA
</commit_message>
<xml_diff>
--- a/LCS_USA_2019.xlsx
+++ b/LCS_USA_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648BCCA6-085A-4E0E-A774-A313E94ADB70}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A048116-A6B3-4005-A453-73B4AA1016A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1541,7 +1541,7 @@
   <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2566,7 +2566,7 @@
         <v>25</v>
       </c>
       <c r="C93" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -2577,7 +2577,7 @@
         <v>25</v>
       </c>
       <c r="C94" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -2588,7 +2588,7 @@
         <v>25</v>
       </c>
       <c r="C95" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -2599,7 +2599,7 @@
         <v>26</v>
       </c>
       <c r="C96" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -2610,7 +2610,7 @@
         <v>26</v>
       </c>
       <c r="C97" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -2621,7 +2621,7 @@
         <v>22</v>
       </c>
       <c r="C98" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -2632,7 +2632,7 @@
         <v>22</v>
       </c>
       <c r="C99" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -2643,7 +2643,7 @@
         <v>22</v>
       </c>
       <c r="C100" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -2654,7 +2654,7 @@
         <v>20</v>
       </c>
       <c r="C101" s="79">
-        <v>10</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>